<commit_message>
Added filters and modularised the code
</commit_message>
<xml_diff>
--- a/data/IVR PoC - Scheme Report Sample.xlsx
+++ b/data/IVR PoC - Scheme Report Sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FAF15A-E630-FE4D-ADC5-ECC922E40DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B3A363-FB5E-F34A-B5F1-638D6295795E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{908E7EA2-3C03-144E-AB44-78DB5EAFD3D2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="218">
   <si>
     <t>Sl No</t>
   </si>
@@ -671,6 +671,27 @@
   </si>
   <si>
     <t>Non Functional</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Div 1</t>
+  </si>
+  <si>
+    <t>Div 2</t>
+  </si>
+  <si>
+    <t>Div 3</t>
+  </si>
+  <si>
+    <t>Div 4</t>
+  </si>
+  <si>
+    <t>Div 5</t>
+  </si>
+  <si>
+    <t>Div 6</t>
   </si>
 </sst>
 </file>
@@ -1578,15 +1599,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42234F0A-8BBC-BE41-A573-3C100EA7986C}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="D18" sqref="D18:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1597,37 +1618,40 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1638,37 +1662,40 @@
         <v>33</v>
       </c>
       <c r="D2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>0.8</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.6</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0.75</v>
       </c>
       <c r="H2" s="1">
         <v>0.75</v>
       </c>
       <c r="I2" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="J2" s="1">
         <v>0.5</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>0.5</v>
       </c>
-      <c r="L2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1679,37 +1706,40 @@
         <v>33</v>
       </c>
       <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>0.6</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.4</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.67</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>0.33</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1720,37 +1750,40 @@
         <v>33</v>
       </c>
       <c r="D4" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>0.56000000000000005</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.83</v>
       </c>
       <c r="G4" s="1">
         <v>0.83</v>
       </c>
       <c r="H4" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="I4" s="1">
         <v>0.6</v>
       </c>
-      <c r="I4" s="1">
+      <c r="J4" s="1">
         <v>0.2</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0.4</v>
       </c>
       <c r="K4" s="1">
         <v>0.4</v>
       </c>
       <c r="L4" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1761,37 +1794,40 @@
         <v>33</v>
       </c>
       <c r="D5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" t="s">
         <v>43</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
       </c>
       <c r="F5" s="1">
         <v>1</v>
       </c>
       <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1">
         <v>0.75</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
       </c>
       <c r="I5" s="1">
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
         <v>1</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1802,10 +1838,10 @@
         <v>33</v>
       </c>
       <c r="D6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1814,25 +1850,28 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="I6" s="1">
         <v>0.33</v>
       </c>
       <c r="J6" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="K6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>0.67</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>1</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>0.54</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1843,37 +1882,40 @@
         <v>34</v>
       </c>
       <c r="D7" t="s">
+        <v>213</v>
+      </c>
+      <c r="E7" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>0.6</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.44</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>0.43</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>0.5</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <v>0.17</v>
       </c>
-      <c r="K7" s="1">
+      <c r="L7" s="1">
         <v>0.33</v>
       </c>
-      <c r="L7" s="1">
+      <c r="M7" s="1">
         <v>1</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>0.75</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1884,37 +1926,40 @@
         <v>34</v>
       </c>
       <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>0.71</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.8</v>
       </c>
       <c r="G8" s="1">
         <v>0.8</v>
       </c>
       <c r="H8" s="1">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="I8" s="1">
         <v>1</v>
       </c>
       <c r="J8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
         <v>1</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>0.75</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1925,22 +1970,22 @@
         <v>35</v>
       </c>
       <c r="D9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>0.67</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.33</v>
       </c>
       <c r="G9" s="1">
         <v>0.33</v>
       </c>
       <c r="H9" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="I9" s="1">
         <v>0.67</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0.33</v>
       </c>
       <c r="J9" s="1">
         <v>0.33</v>
@@ -1954,8 +1999,11 @@
       <c r="M9" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1966,16 +2014,16 @@
         <v>36</v>
       </c>
       <c r="D10" t="s">
+        <v>214</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>0.86</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.8</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0.67</v>
       </c>
       <c r="H10" s="1">
         <v>0.67</v>
@@ -1984,19 +2032,22 @@
         <v>0.67</v>
       </c>
       <c r="J10" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="1">
+      <c r="L10" s="1">
         <v>0.33</v>
-      </c>
-      <c r="L10" s="1">
-        <v>0.67</v>
       </c>
       <c r="M10" s="1">
         <v>0.67</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N10" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2007,37 +2058,40 @@
         <v>37</v>
       </c>
       <c r="D11" t="s">
+        <v>214</v>
+      </c>
+      <c r="E11" t="s">
         <v>45</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0.4</v>
       </c>
       <c r="F11" s="1">
         <v>0.4</v>
       </c>
       <c r="G11" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="H11" s="1">
         <v>0.2</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>0.75</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0.25</v>
       </c>
       <c r="J11" s="1">
         <v>0.25</v>
       </c>
       <c r="K11" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="L11" s="1">
         <v>0.5</v>
       </c>
-      <c r="L11" s="1">
+      <c r="M11" s="1">
         <v>0.33</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>0.31</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2048,10 +2102,10 @@
         <v>37</v>
       </c>
       <c r="D12" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" t="s">
         <v>45</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -2060,25 +2114,28 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="I12" s="1">
         <v>0.33</v>
       </c>
       <c r="J12" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
+      <c r="L12" s="1">
         <v>0.67</v>
       </c>
-      <c r="L12" s="1">
+      <c r="M12" s="1">
         <v>0.33</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>0.31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2089,37 +2146,40 @@
         <v>37</v>
       </c>
       <c r="D13" t="s">
+        <v>214</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0.33</v>
       </c>
       <c r="F13" s="1">
         <v>0.33</v>
       </c>
       <c r="G13" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="H13" s="1">
         <v>0.67</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0.33</v>
       </c>
       <c r="I13" s="1">
         <v>0.33</v>
       </c>
       <c r="J13" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="K13" s="1">
+      <c r="L13" s="1">
         <v>0.67</v>
       </c>
-      <c r="L13" s="1">
+      <c r="M13" s="1">
         <v>0.33</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>0.31</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2130,37 +2190,40 @@
         <v>38</v>
       </c>
       <c r="D14" t="s">
+        <v>215</v>
+      </c>
+      <c r="E14" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>0.5</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.38</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>0.71</v>
-      </c>
-      <c r="I14" s="1">
-        <v>0.43</v>
       </c>
       <c r="J14" s="1">
         <v>0.43</v>
       </c>
       <c r="K14" s="1">
+        <v>0.43</v>
+      </c>
+      <c r="L14" s="1">
         <v>0.14000000000000001</v>
-      </c>
-      <c r="L14" s="1">
-        <v>0.43</v>
       </c>
       <c r="M14" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N14" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2171,37 +2234,40 @@
         <v>39</v>
       </c>
       <c r="D15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E15" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>0.88</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>1</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>0.6</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>0.75</v>
-      </c>
-      <c r="I15" s="1">
-        <v>0.5</v>
       </c>
       <c r="J15" s="1">
         <v>0.5</v>
       </c>
       <c r="K15" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="L15" s="1">
         <v>0</v>
       </c>
-      <c r="L15" s="1">
+      <c r="M15" s="1">
         <v>0.5</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>0.42</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2212,22 +2278,22 @@
         <v>39</v>
       </c>
       <c r="D16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>0.25</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>0.5</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0.67</v>
       </c>
       <c r="H16" s="1">
         <v>0.67</v>
       </c>
       <c r="I16" s="1">
-        <v>0.33</v>
+        <v>0.67</v>
       </c>
       <c r="J16" s="1">
         <v>0.33</v>
@@ -2236,13 +2302,16 @@
         <v>0.33</v>
       </c>
       <c r="L16" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="M16" s="1">
         <v>0.5</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>0.42</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2252,38 +2321,41 @@
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>0.45</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>0.43</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>0.8</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>0.6</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0.2</v>
       </c>
       <c r="K17" s="1">
         <v>0.2</v>
       </c>
       <c r="L17" s="1">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="M17" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N17" s="1">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2293,11 +2365,11 @@
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E18" t="s">
         <v>47</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
       </c>
       <c r="F18" s="1">
         <v>1</v>
@@ -2312,19 +2384,22 @@
         <v>1</v>
       </c>
       <c r="J18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="1">
         <v>0</v>
       </c>
       <c r="L18" s="1">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1">
         <v>1</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>0.63</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2334,38 +2409,41 @@
       <c r="C19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E19" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>0.8</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>0.75</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
       </c>
       <c r="H19" s="1">
         <v>1</v>
       </c>
       <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
         <v>0.25</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K19" s="1">
         <v>0.75</v>
       </c>
-      <c r="K19" s="1">
+      <c r="L19" s="1">
         <v>0</v>
       </c>
-      <c r="L19" s="1">
+      <c r="M19" s="1">
         <v>1</v>
       </c>
-      <c r="M19" s="1">
+      <c r="N19" s="1">
         <v>0.63</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2375,38 +2453,41 @@
       <c r="C20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E20" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>0.4</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>0.5</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>0.33</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>0</v>
       </c>
-      <c r="J20" s="1">
+      <c r="K20" s="1">
         <v>0.67</v>
-      </c>
-      <c r="K20" s="1">
-        <v>0.33</v>
       </c>
       <c r="L20" s="1">
         <v>0.33</v>
       </c>
       <c r="M20" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="N20" s="1">
         <v>0.17</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2416,34 +2497,37 @@
       <c r="C21" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E21" t="s">
         <v>47</v>
-      </c>
-      <c r="E21" s="1">
-        <v>1</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
       </c>
       <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1">
         <v>0.8</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>1</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>0.33</v>
       </c>
-      <c r="J21" s="1">
+      <c r="K21" s="1">
         <v>0.67</v>
       </c>
-      <c r="K21" s="1">
+      <c r="L21" s="1">
         <v>0</v>
       </c>
-      <c r="L21" s="1">
+      <c r="M21" s="1">
         <v>0.33</v>
       </c>
-      <c r="M21" s="1">
+      <c r="N21" s="1">
         <v>0.17</v>
       </c>
     </row>
@@ -4354,7 +4438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5EDA552-1483-C340-B473-004D9606835C}">
   <dimension ref="B1:H141"/>
   <sheetViews>
-    <sheetView topLeftCell="A56" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>

</xml_diff>